<commit_message>
Skeleton for download Excel.
</commit_message>
<xml_diff>
--- a/source/goodway/goodway-web2/src/main/resources/excel-templates/Template_Question.xlsx
+++ b/source/goodway/goodway-web2/src/main/resources/excel-templates/Template_Question.xlsx
@@ -19,6 +19,29 @@
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Windows User</author>
+  </authors>
+  <commentList>
+    <comment ref="E7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>question</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -103,7 +126,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -129,6 +152,12 @@
       <b/>
       <sz val="12"/>
       <color indexed="9"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -250,20 +279,8 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -300,683 +317,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="204">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="108">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2032,352 +1389,352 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="39.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="54" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="20" style="2" customWidth="1"/>
-    <col min="12" max="13" width="17" style="2" customWidth="1"/>
-    <col min="14" max="15" width="20.42578125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="22.42578125" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="4" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="54" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20" style="1" customWidth="1"/>
+    <col min="12" max="13" width="17" style="1" customWidth="1"/>
+    <col min="14" max="15" width="20.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="22.42578125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2">
+      <c r="B1" s="15"/>
+      <c r="C1" s="1">
         <f>COUNTIF(J:J, "Open")</f>
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="2">
+      <c r="B2" s="16"/>
+      <c r="C2" s="1">
         <f>COUNTIF(J:J, "In progress")</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="2">
+      <c r="B3" s="17"/>
+      <c r="C3" s="1">
         <f>COUNTIF(J:J, "Closed")</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="2">
+      <c r="B4" s="17"/>
+      <c r="C4" s="1">
         <f>COUNTIF(J:J, "Canceled")</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="2">
+      <c r="B5" s="18"/>
+      <c r="C5" s="1">
         <f>SUM(C1:C4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="M7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="N7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="O7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P7" s="7" t="s">
+      <c r="P7" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="13" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
+    <row r="8" spans="1:16" s="9" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
         <v>1</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="10"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="6"/>
     </row>
-    <row r="9" spans="1:16" s="13" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9">
+    <row r="9" spans="1:16" s="9" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
         <v>2</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="10"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="6"/>
     </row>
-    <row r="10" spans="1:16" s="13" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
+    <row r="10" spans="1:16" s="9" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
         <v>3</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="10"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="6"/>
     </row>
-    <row r="11" spans="1:16" s="13" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
+    <row r="11" spans="1:16" s="9" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
         <v>4</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="10"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="6"/>
     </row>
-    <row r="12" spans="1:16" s="13" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
+    <row r="12" spans="1:16" s="9" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
         <v>5</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="10"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="6"/>
     </row>
-    <row r="13" spans="1:16" s="13" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
+    <row r="13" spans="1:16" s="9" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
         <v>6</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="10"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="6"/>
     </row>
-    <row r="14" spans="1:16" s="13" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9">
+    <row r="14" spans="1:16" s="9" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
         <v>7</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="10"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="6"/>
     </row>
-    <row r="15" spans="1:16" s="13" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
+    <row r="15" spans="1:16" s="9" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
         <v>8</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="10"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="6"/>
     </row>
-    <row r="16" spans="1:16" s="13" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
+    <row r="16" spans="1:16" s="9" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
         <v>9</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="10"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="6"/>
     </row>
-    <row r="17" spans="1:16" s="13" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
+    <row r="17" spans="1:16" s="9" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
         <v>10</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="10"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="6"/>
     </row>
-    <row r="18" spans="1:16" s="13" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
+    <row r="18" spans="1:16" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
     </row>
     <row r="19" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -2390,387 +1747,387 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="P8:P9 N8:N9 O8 A8:F8 C9:G9 G11:G15 G8:M10 A9:B15 I11:K16">
-    <cfRule type="expression" dxfId="203" priority="223" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="223" stopIfTrue="1">
       <formula>($J8="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="202" priority="224" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="224" stopIfTrue="1">
       <formula>($J8="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="201" priority="225" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="225" stopIfTrue="1">
       <formula>($J8="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:F11 P10:P11 N10:N11 F15:F17 P15:P16 N15:N16">
-    <cfRule type="expression" dxfId="200" priority="226" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="226" stopIfTrue="1">
       <formula>($J9="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="199" priority="227" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="227" stopIfTrue="1">
       <formula>($J9="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="198" priority="228" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="228" stopIfTrue="1">
       <formula>($J9="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="197" priority="220" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="220" stopIfTrue="1">
       <formula>($J10="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="196" priority="221" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="221" stopIfTrue="1">
       <formula>($J10="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="195" priority="222" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="222" stopIfTrue="1">
       <formula>($J10="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="expression" dxfId="194" priority="217" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="217" stopIfTrue="1">
       <formula>($J10="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="193" priority="218" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="218" stopIfTrue="1">
       <formula>($J10="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="192" priority="219" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="219" stopIfTrue="1">
       <formula>($J10="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="expression" dxfId="191" priority="214" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="214" stopIfTrue="1">
       <formula>($J10="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="190" priority="215" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="215" stopIfTrue="1">
       <formula>($J10="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="189" priority="216" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="216" stopIfTrue="1">
       <formula>($J10="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9">
-    <cfRule type="expression" dxfId="188" priority="211" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="211" stopIfTrue="1">
       <formula>($J9="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="187" priority="212" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="212" stopIfTrue="1">
       <formula>($J9="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="186" priority="213" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="213" stopIfTrue="1">
       <formula>($J9="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11 H11 L11:M11">
-    <cfRule type="expression" dxfId="185" priority="205" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="205" stopIfTrue="1">
       <formula>($J11="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="184" priority="206" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="206" stopIfTrue="1">
       <formula>($J11="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="183" priority="207" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="207" stopIfTrue="1">
       <formula>($J11="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="182" priority="202" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="202" stopIfTrue="1">
       <formula>($J11="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="181" priority="203" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="203" stopIfTrue="1">
       <formula>($J11="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="180" priority="204" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="204" stopIfTrue="1">
       <formula>($J11="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="179" priority="199" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="199" stopIfTrue="1">
       <formula>($J11="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="178" priority="200" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="200" stopIfTrue="1">
       <formula>($J11="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="177" priority="201" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="201" stopIfTrue="1">
       <formula>($J11="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="expression" dxfId="176" priority="196" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="196" stopIfTrue="1">
       <formula>($J11="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="175" priority="197" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="197" stopIfTrue="1">
       <formula>($J11="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="198" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="198" stopIfTrue="1">
       <formula>($J11="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12 P12 N12">
-    <cfRule type="expression" dxfId="173" priority="193" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="193" stopIfTrue="1">
       <formula>($J11="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="172" priority="194" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="194" stopIfTrue="1">
       <formula>($J11="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="171" priority="195" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="195" stopIfTrue="1">
       <formula>($J11="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12 O12 L12:M12">
-    <cfRule type="expression" dxfId="170" priority="190" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="190" stopIfTrue="1">
       <formula>($J12="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="169" priority="191" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="191" stopIfTrue="1">
       <formula>($J12="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="168" priority="192" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="192" stopIfTrue="1">
       <formula>($J12="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="167" priority="187" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="187" stopIfTrue="1">
       <formula>($J12="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="188" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="188" stopIfTrue="1">
       <formula>($J12="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="165" priority="189" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="189" stopIfTrue="1">
       <formula>($J12="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="164" priority="184" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="184" stopIfTrue="1">
       <formula>($J12="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="163" priority="185" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="185" stopIfTrue="1">
       <formula>($J12="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="186" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="186" stopIfTrue="1">
       <formula>($J12="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="expression" dxfId="161" priority="181" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="181" stopIfTrue="1">
       <formula>($J12="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="182" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="182" stopIfTrue="1">
       <formula>($J12="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="159" priority="183" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="183" stopIfTrue="1">
       <formula>($J12="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13 P13 N13">
-    <cfRule type="expression" dxfId="158" priority="175" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="175" stopIfTrue="1">
       <formula>($J12="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="157" priority="176" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="176" stopIfTrue="1">
       <formula>($J12="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="177" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="177" stopIfTrue="1">
       <formula>($J12="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13 O13 L13:M13">
-    <cfRule type="expression" dxfId="155" priority="172" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="172" stopIfTrue="1">
       <formula>($J13="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="173" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="173" stopIfTrue="1">
       <formula>($J13="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="153" priority="174" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="174" stopIfTrue="1">
       <formula>($J13="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="152" priority="169" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="169" stopIfTrue="1">
       <formula>($J13="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="151" priority="170" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="170" stopIfTrue="1">
       <formula>($J13="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="150" priority="171" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="171" stopIfTrue="1">
       <formula>($J13="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="149" priority="166" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="166" stopIfTrue="1">
       <formula>($J13="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="167" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="167" stopIfTrue="1">
       <formula>($J13="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="147" priority="168" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="168" stopIfTrue="1">
       <formula>($J13="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="146" priority="163" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="163" stopIfTrue="1">
       <formula>($J13="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="145" priority="164" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="164" stopIfTrue="1">
       <formula>($J13="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="165" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="165" stopIfTrue="1">
       <formula>($J13="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14 P14 N14">
-    <cfRule type="expression" dxfId="143" priority="157" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="157" stopIfTrue="1">
       <formula>($J13="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="158" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="158" stopIfTrue="1">
       <formula>($J13="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="141" priority="159" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="159" stopIfTrue="1">
       <formula>($J13="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14 O14 L14:M14">
-    <cfRule type="expression" dxfId="140" priority="154" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="154" stopIfTrue="1">
       <formula>($J14="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="155" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="155" stopIfTrue="1">
       <formula>($J14="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="156" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="156" stopIfTrue="1">
       <formula>($J14="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="137" priority="151" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="151" stopIfTrue="1">
       <formula>($J14="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="152" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="152" stopIfTrue="1">
       <formula>($J14="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="135" priority="153" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="153" stopIfTrue="1">
       <formula>($J14="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="134" priority="148" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="148" stopIfTrue="1">
       <formula>($J14="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="133" priority="149" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="149" stopIfTrue="1">
       <formula>($J14="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="150" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="150" stopIfTrue="1">
       <formula>($J14="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="131" priority="145" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="145" stopIfTrue="1">
       <formula>($J14="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="130" priority="146" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="146" stopIfTrue="1">
       <formula>($J14="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="147" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="147" stopIfTrue="1">
       <formula>($J14="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:H16 O15 L15:M16">
-    <cfRule type="expression" dxfId="128" priority="136" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="136" stopIfTrue="1">
       <formula>($J15="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="127" priority="137" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="137" stopIfTrue="1">
       <formula>($J15="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="138" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="138" stopIfTrue="1">
       <formula>($J15="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="125" priority="133" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="133" stopIfTrue="1">
       <formula>($J15="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="134" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="134" stopIfTrue="1">
       <formula>($J15="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="135" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="135" stopIfTrue="1">
       <formula>($J15="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="122" priority="130" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="130" stopIfTrue="1">
       <formula>($J15="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="131" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="131" stopIfTrue="1">
       <formula>($J15="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="132" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="132" stopIfTrue="1">
       <formula>($J15="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="119" priority="127" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="127" stopIfTrue="1">
       <formula>($J15="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="128" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="128" stopIfTrue="1">
       <formula>($J15="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="129" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="129" stopIfTrue="1">
       <formula>($J15="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O10">
-    <cfRule type="expression" dxfId="116" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="94" stopIfTrue="1">
       <formula>($J10="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="95" stopIfTrue="1">
       <formula>($J10="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="96" stopIfTrue="1">
       <formula>($J10="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="expression" dxfId="110" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="88" stopIfTrue="1">
       <formula>($J16="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="89" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="89" stopIfTrue="1">
       <formula>($J16="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="90" stopIfTrue="1">
       <formula>($J16="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O16">
-    <cfRule type="expression" dxfId="107" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="85" stopIfTrue="1">
       <formula>($J16="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="86" stopIfTrue="1">
       <formula>($J16="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="87" stopIfTrue="1">
       <formula>($J16="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O17 G17:M17">
-    <cfRule type="expression" dxfId="26" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="22" stopIfTrue="1">
       <formula>($J17="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="23" stopIfTrue="1">
       <formula>($J17="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="24" stopIfTrue="1">
       <formula>($J17="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17 N17">
-    <cfRule type="expression" dxfId="23" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="19" stopIfTrue="1">
       <formula>($J4="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="20" stopIfTrue="1">
       <formula>($J4="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="21" stopIfTrue="1">
       <formula>($J4="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:E17">
-    <cfRule type="expression" dxfId="20" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="16" stopIfTrue="1">
       <formula>($J18="In Progress")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="17" stopIfTrue="1">
       <formula>($J18="Closed")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="18" stopIfTrue="1">
       <formula>($J18="Canceled")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2804,5 +2161,6 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L14e-BM/PM/HDCV/G8-HSK v1/2&amp;CInternal use&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>